<commit_message>
add comments with units and correct types and string lengths
</commit_message>
<xml_diff>
--- a/testlab-db/neware_database_master2.xlsx
+++ b/testlab-db/neware_database_master2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://basquevolt-my.sharepoint.com/personal/ecalandrini_basquevolt_com/Documents/Documents/Lavoro/Software/NewareDB/testlab-db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="394" documentId="8_{F5CC27F1-63FB-4B55-A392-FA796873BBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46276A4B-E17D-4221-9755-05CEF8456E6C}"/>
+  <xr:revisionPtr revIDLastSave="418" documentId="8_{F5CC27F1-63FB-4B55-A392-FA796873BBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB434443-B0FD-4E26-BF07-316D3013C5C7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{F9E3BB05-05FB-4358-BC5E-97EF2B4FB956}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1697" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1703" uniqueCount="455">
   <si>
     <t>computer_name</t>
   </si>
@@ -1625,7 +1625,7 @@
   <autoFilter ref="A1:K210" xr:uid="{2AF3C50B-29E8-4820-8C07-E4AE3DEFB3B3}">
     <filterColumn colId="0">
       <filters>
-        <filter val="log"/>
+        <filter val="step"/>
       </filters>
     </filterColumn>
     <filterColumn colId="1">
@@ -8571,7 +8571,7 @@
   <dimension ref="A1:K210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C220" sqref="C220"/>
+      <selection activeCell="H153" sqref="H153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10822,7 +10822,9 @@
         <v>443</v>
       </c>
       <c r="J79" s="2"/>
-      <c r="K79" s="4"/>
+      <c r="K79" s="4" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
@@ -11484,7 +11486,9 @@
         <v>443</v>
       </c>
       <c r="J103" s="2"/>
-      <c r="K103" s="4"/>
+      <c r="K103" s="2" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
@@ -11630,7 +11634,9 @@
       <c r="D109" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E109" s="2"/>
+      <c r="E109" s="2">
+        <v>4</v>
+      </c>
       <c r="F109" s="2" t="s">
         <v>129</v>
       </c>
@@ -11657,7 +11663,9 @@
       <c r="D110" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="E110" s="2"/>
+      <c r="E110" s="2">
+        <v>4</v>
+      </c>
       <c r="F110" s="2" t="s">
         <v>129</v>
       </c>
@@ -11682,7 +11690,9 @@
       <c r="D111" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="E111" s="2"/>
+      <c r="E111" s="2">
+        <v>4</v>
+      </c>
       <c r="F111" s="2" t="s">
         <v>129</v>
       </c>
@@ -11707,7 +11717,9 @@
       <c r="D112" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="E112" s="2"/>
+      <c r="E112" s="2">
+        <v>4</v>
+      </c>
       <c r="F112" s="2" t="s">
         <v>129</v>
       </c>
@@ -11730,7 +11742,9 @@
         <v>378</v>
       </c>
       <c r="D113" s="2"/>
-      <c r="E113" s="2"/>
+      <c r="E113" s="2">
+        <v>4</v>
+      </c>
       <c r="F113" s="2" t="s">
         <v>129</v>
       </c>
@@ -11755,7 +11769,9 @@
       <c r="D114" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E114" s="2"/>
+      <c r="E114" s="2">
+        <v>4</v>
+      </c>
       <c r="F114" s="2" t="s">
         <v>129</v>
       </c>
@@ -11772,7 +11788,7 @@
         <v>44</v>
       </c>
       <c r="B115" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>380</v>
@@ -11780,7 +11796,9 @@
       <c r="D115" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E115" s="2"/>
+      <c r="E115" s="2">
+        <v>4</v>
+      </c>
       <c r="F115" s="2" t="s">
         <v>131</v>
       </c>
@@ -11805,7 +11823,9 @@
       <c r="D116" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E116" s="2"/>
+      <c r="E116" s="2">
+        <v>4</v>
+      </c>
       <c r="F116" s="2" t="s">
         <v>129</v>
       </c>
@@ -11830,7 +11850,9 @@
       <c r="D117" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E117" s="2"/>
+      <c r="E117" s="2">
+        <v>4</v>
+      </c>
       <c r="F117" s="2" t="s">
         <v>131</v>
       </c>
@@ -11857,7 +11879,9 @@
       <c r="D118" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E118" s="2"/>
+      <c r="E118" s="2">
+        <v>4</v>
+      </c>
       <c r="F118" s="2" t="s">
         <v>129</v>
       </c>
@@ -11882,7 +11906,9 @@
       <c r="D119" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E119" s="2"/>
+      <c r="E119" s="2">
+        <v>4</v>
+      </c>
       <c r="F119" s="2" t="s">
         <v>131</v>
       </c>
@@ -11909,7 +11935,9 @@
       <c r="D120" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E120" s="2"/>
+      <c r="E120" s="2">
+        <v>4</v>
+      </c>
       <c r="F120" s="2" t="s">
         <v>129</v>
       </c>
@@ -11934,7 +11962,9 @@
       <c r="D121" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E121" s="2"/>
+      <c r="E121" s="2">
+        <v>4</v>
+      </c>
       <c r="F121" s="2" t="s">
         <v>131</v>
       </c>
@@ -11961,7 +11991,9 @@
       <c r="D122" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E122" s="2"/>
+      <c r="E122" s="2">
+        <v>4</v>
+      </c>
       <c r="F122" s="2" t="s">
         <v>129</v>
       </c>
@@ -11983,8 +12015,12 @@
       <c r="C123" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="D123" s="2"/>
-      <c r="E123" s="2"/>
+      <c r="D123" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E123" s="2">
+        <v>4</v>
+      </c>
       <c r="F123" s="2" t="s">
         <v>131</v>
       </c>
@@ -12008,8 +12044,12 @@
       <c r="C124" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="D124" s="2"/>
-      <c r="E124" s="2"/>
+      <c r="D124" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E124" s="2">
+        <v>4</v>
+      </c>
       <c r="F124" s="2" t="s">
         <v>131</v>
       </c>
@@ -12033,8 +12073,12 @@
       <c r="C125" s="4" t="s">
         <v>393</v>
       </c>
-      <c r="D125" s="2"/>
-      <c r="E125" s="2"/>
+      <c r="D125" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E125" s="2">
+        <v>4</v>
+      </c>
       <c r="F125" s="2" t="s">
         <v>131</v>
       </c>
@@ -12058,8 +12102,12 @@
       <c r="C126" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="D126" s="2"/>
-      <c r="E126" s="2"/>
+      <c r="D126" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="E126" s="2">
+        <v>4</v>
+      </c>
       <c r="F126" s="2" t="s">
         <v>131</v>
       </c>
@@ -12073,7 +12121,7 @@
       <c r="J126" s="2"/>
       <c r="K126" s="4"/>
     </row>
-    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>54</v>
       </c>
@@ -12098,7 +12146,7 @@
       </c>
       <c r="K127" s="4"/>
     </row>
-    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>54</v>
       </c>
@@ -12121,7 +12169,7 @@
       <c r="J128" s="2"/>
       <c r="K128" s="4"/>
     </row>
-    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>54</v>
       </c>
@@ -12146,7 +12194,7 @@
       <c r="J129" s="2"/>
       <c r="K129" s="4"/>
     </row>
-    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>54</v>
       </c>
@@ -12173,7 +12221,7 @@
       <c r="J130" s="2"/>
       <c r="K130" s="4"/>
     </row>
-    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>54</v>
       </c>
@@ -12202,7 +12250,7 @@
       </c>
       <c r="K131" s="4"/>
     </row>
-    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>54</v>
       </c>
@@ -12227,7 +12275,7 @@
       <c r="J132" s="2"/>
       <c r="K132" s="4"/>
     </row>
-    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>54</v>
       </c>
@@ -12252,7 +12300,7 @@
       <c r="J133" s="2"/>
       <c r="K133" s="4"/>
     </row>
-    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>54</v>
       </c>
@@ -12277,7 +12325,7 @@
       <c r="J134" s="2"/>
       <c r="K134" s="4"/>
     </row>
-    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>54</v>
       </c>
@@ -12306,7 +12354,7 @@
       <c r="J135" s="2"/>
       <c r="K135" s="4"/>
     </row>
-    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>54</v>
       </c>
@@ -12337,7 +12385,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>54</v>
       </c>
@@ -12364,7 +12412,7 @@
       <c r="J137" s="2"/>
       <c r="K137" s="4"/>
     </row>
-    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>54</v>
       </c>
@@ -12395,7 +12443,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>54</v>
       </c>
@@ -12455,7 +12503,7 @@
       <c r="J140" s="2"/>
       <c r="K140" s="4"/>
     </row>
-    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>54</v>
       </c>
@@ -12486,7 +12534,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>54</v>
       </c>
@@ -12546,7 +12594,7 @@
       <c r="J143" s="2"/>
       <c r="K143" s="4"/>
     </row>
-    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>54</v>
       </c>
@@ -12577,7 +12625,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>54</v>
       </c>
@@ -12608,7 +12656,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>54</v>
       </c>
@@ -12639,7 +12687,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>54</v>
       </c>
@@ -12670,7 +12718,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>54</v>
       </c>
@@ -12699,7 +12747,7 @@
       <c r="J148" s="2"/>
       <c r="K148" s="4"/>
     </row>
-    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>54</v>
       </c>
@@ -12728,7 +12776,7 @@
       <c r="J149" s="2"/>
       <c r="K149" s="4"/>
     </row>
-    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>54</v>
       </c>
@@ -12757,7 +12805,7 @@
       <c r="J150" s="2"/>
       <c r="K150" s="4"/>
     </row>
-    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>54</v>
       </c>
@@ -12784,7 +12832,7 @@
       <c r="J151" s="2"/>
       <c r="K151" s="4"/>
     </row>
-    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>54</v>
       </c>
@@ -12811,7 +12859,7 @@
       <c r="J152" s="2"/>
       <c r="K152" s="4"/>
     </row>
-    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>54</v>
       </c>
@@ -12838,7 +12886,7 @@
       <c r="J153" s="2"/>
       <c r="K153" s="4"/>
     </row>
-    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>54</v>
       </c>
@@ -12865,7 +12913,7 @@
       <c r="J154" s="2"/>
       <c r="K154" s="4"/>
     </row>
-    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>54</v>
       </c>
@@ -12892,7 +12940,7 @@
       <c r="J155" s="2"/>
       <c r="K155" s="4"/>
     </row>
-    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>54</v>
       </c>
@@ -12942,7 +12990,7 @@
       <c r="J157" s="2"/>
       <c r="K157" s="4"/>
     </row>
-    <row r="158" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>54</v>
       </c>
@@ -12969,7 +13017,7 @@
       <c r="J158" s="2"/>
       <c r="K158" s="4"/>
     </row>
-    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>54</v>
       </c>
@@ -12996,7 +13044,7 @@
       <c r="J159" s="2"/>
       <c r="K159" s="4"/>
     </row>
-    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>54</v>
       </c>
@@ -13023,7 +13071,7 @@
       <c r="J160" s="2"/>
       <c r="K160" s="4"/>
     </row>
-    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>54</v>
       </c>
@@ -13123,7 +13171,7 @@
       <c r="J164" s="2"/>
       <c r="K164" s="4"/>
     </row>
-    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>54</v>
       </c>
@@ -13152,7 +13200,7 @@
       <c r="J165" s="2"/>
       <c r="K165" s="4"/>
     </row>
-    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>54</v>
       </c>
@@ -13181,7 +13229,7 @@
       <c r="J166" s="2"/>
       <c r="K166" s="4"/>
     </row>
-    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>54</v>
       </c>
@@ -14091,7 +14139,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>137</v>
       </c>
@@ -14116,7 +14164,7 @@
       </c>
       <c r="K201" s="4"/>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>137</v>
       </c>
@@ -14139,7 +14187,7 @@
       <c r="J202" s="2"/>
       <c r="K202" s="4"/>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>137</v>
       </c>
@@ -14164,7 +14212,7 @@
       <c r="J203" s="2"/>
       <c r="K203" s="4"/>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>137</v>
       </c>
@@ -14191,7 +14239,7 @@
       <c r="J204" s="2"/>
       <c r="K204" s="4"/>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>137</v>
       </c>
@@ -14218,7 +14266,7 @@
       <c r="J205" s="2"/>
       <c r="K205" s="4"/>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>137</v>
       </c>
@@ -14247,7 +14295,7 @@
       </c>
       <c r="K206" s="4"/>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>137</v>
       </c>
@@ -14274,7 +14322,7 @@
       <c r="J207" s="2"/>
       <c r="K207" s="4"/>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>137</v>
       </c>
@@ -14301,7 +14349,7 @@
       <c r="J208" s="2"/>
       <c r="K208" s="4"/>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>137</v>
       </c>
@@ -14328,7 +14376,7 @@
       <c r="J209" s="2"/>
       <c r="K209" s="4"/>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
created folder with database configuration file
</commit_message>
<xml_diff>
--- a/testlab-db/neware_database_master2.xlsx
+++ b/testlab-db/neware_database_master2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://basquevolt-my.sharepoint.com/personal/ecalandrini_basquevolt_com/Documents/Documents/Lavoro/Software/NewareDB/testlab-db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="418" documentId="8_{F5CC27F1-63FB-4B55-A392-FA796873BBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB434443-B0FD-4E26-BF07-316D3013C5C7}"/>
+  <xr:revisionPtr revIDLastSave="440" documentId="8_{F5CC27F1-63FB-4B55-A392-FA796873BBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A28ADC2B-3096-4B70-B8AA-E978A45D5431}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{F9E3BB05-05FB-4358-BC5E-97EF2B4FB956}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="21810" windowHeight="20970" activeTab="1" xr2:uid="{F9E3BB05-05FB-4358-BC5E-97EF2B4FB956}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1703" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="458">
   <si>
     <t>computer_name</t>
   </si>
@@ -1414,6 +1414,15 @@
   </si>
   <si>
     <t>`150</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> aux_single_voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> aux_single_temperature</t>
+  </si>
+  <si>
+    <t>aux_temperature</t>
   </si>
 </sst>
 </file>
@@ -1625,12 +1634,7 @@
   <autoFilter ref="A1:K210" xr:uid="{2AF3C50B-29E8-4820-8C07-E4AE3DEFB3B3}">
     <filterColumn colId="0">
       <filters>
-        <filter val="step"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="1">
-      <filters>
-        <filter val="TRUE"/>
+        <filter val="log"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1970,8 +1974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E231686A-ED7E-47C8-99ED-C3B9B1E077F6}">
   <dimension ref="A1:W187"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:R1048576"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106:A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8571,7 +8575,7 @@
   <dimension ref="A1:K210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H153" sqref="H153"/>
+      <selection activeCell="E186" sqref="E186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9725,7 +9729,7 @@
       </c>
       <c r="J39" s="2"/>
       <c r="K39" s="2" t="s">
-        <v>111</v>
+        <v>455</v>
       </c>
     </row>
     <row r="40" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -9756,7 +9760,7 @@
       </c>
       <c r="J40" s="2"/>
       <c r="K40" s="2" t="s">
-        <v>112</v>
+        <v>456</v>
       </c>
     </row>
     <row r="41" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
@@ -11842,7 +11846,7 @@
         <v>44</v>
       </c>
       <c r="B117" s="4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>382</v>
@@ -12121,7 +12125,7 @@
       <c r="J126" s="2"/>
       <c r="K126" s="4"/>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>54</v>
       </c>
@@ -12146,7 +12150,7 @@
       </c>
       <c r="K127" s="4"/>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>54</v>
       </c>
@@ -12169,7 +12173,7 @@
       <c r="J128" s="2"/>
       <c r="K128" s="4"/>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>54</v>
       </c>
@@ -12194,7 +12198,7 @@
       <c r="J129" s="2"/>
       <c r="K129" s="4"/>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>54</v>
       </c>
@@ -12221,7 +12225,7 @@
       <c r="J130" s="2"/>
       <c r="K130" s="4"/>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>54</v>
       </c>
@@ -12250,7 +12254,7 @@
       </c>
       <c r="K131" s="4"/>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>54</v>
       </c>
@@ -12275,7 +12279,7 @@
       <c r="J132" s="2"/>
       <c r="K132" s="4"/>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>54</v>
       </c>
@@ -12300,7 +12304,7 @@
       <c r="J133" s="2"/>
       <c r="K133" s="4"/>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>54</v>
       </c>
@@ -12325,7 +12329,7 @@
       <c r="J134" s="2"/>
       <c r="K134" s="4"/>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>54</v>
       </c>
@@ -12354,7 +12358,7 @@
       <c r="J135" s="2"/>
       <c r="K135" s="4"/>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>54</v>
       </c>
@@ -12385,7 +12389,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>54</v>
       </c>
@@ -12412,7 +12416,7 @@
       <c r="J137" s="2"/>
       <c r="K137" s="4"/>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>54</v>
       </c>
@@ -12443,7 +12447,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>54</v>
       </c>
@@ -12503,7 +12507,7 @@
       <c r="J140" s="2"/>
       <c r="K140" s="4"/>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>54</v>
       </c>
@@ -12534,7 +12538,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>54</v>
       </c>
@@ -12594,7 +12598,7 @@
       <c r="J143" s="2"/>
       <c r="K143" s="4"/>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>54</v>
       </c>
@@ -12625,7 +12629,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>54</v>
       </c>
@@ -12656,7 +12660,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>54</v>
       </c>
@@ -12687,7 +12691,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>54</v>
       </c>
@@ -12718,7 +12722,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>54</v>
       </c>
@@ -12747,7 +12751,7 @@
       <c r="J148" s="2"/>
       <c r="K148" s="4"/>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>54</v>
       </c>
@@ -12776,7 +12780,7 @@
       <c r="J149" s="2"/>
       <c r="K149" s="4"/>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>54</v>
       </c>
@@ -12805,7 +12809,7 @@
       <c r="J150" s="2"/>
       <c r="K150" s="4"/>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>54</v>
       </c>
@@ -12832,7 +12836,7 @@
       <c r="J151" s="2"/>
       <c r="K151" s="4"/>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>54</v>
       </c>
@@ -12859,7 +12863,7 @@
       <c r="J152" s="2"/>
       <c r="K152" s="4"/>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>54</v>
       </c>
@@ -12886,7 +12890,7 @@
       <c r="J153" s="2"/>
       <c r="K153" s="4"/>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>54</v>
       </c>
@@ -12913,7 +12917,7 @@
       <c r="J154" s="2"/>
       <c r="K154" s="4"/>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>54</v>
       </c>
@@ -12940,7 +12944,7 @@
       <c r="J155" s="2"/>
       <c r="K155" s="4"/>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>54</v>
       </c>
@@ -12990,7 +12994,7 @@
       <c r="J157" s="2"/>
       <c r="K157" s="4"/>
     </row>
-    <row r="158" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>54</v>
       </c>
@@ -13017,7 +13021,7 @@
       <c r="J158" s="2"/>
       <c r="K158" s="4"/>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>54</v>
       </c>
@@ -13044,7 +13048,7 @@
       <c r="J159" s="2"/>
       <c r="K159" s="4"/>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>54</v>
       </c>
@@ -13071,7 +13075,7 @@
       <c r="J160" s="2"/>
       <c r="K160" s="4"/>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>54</v>
       </c>
@@ -13171,7 +13175,7 @@
       <c r="J164" s="2"/>
       <c r="K164" s="4"/>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>54</v>
       </c>
@@ -13200,7 +13204,7 @@
       <c r="J165" s="2"/>
       <c r="K165" s="4"/>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>54</v>
       </c>
@@ -13229,7 +13233,7 @@
       <c r="J166" s="2"/>
       <c r="K166" s="4"/>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>54</v>
       </c>
@@ -13731,7 +13735,7 @@
         <v>271</v>
       </c>
       <c r="E185" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F185" s="2" t="s">
         <v>129</v>
@@ -13746,7 +13750,9 @@
         <v>443</v>
       </c>
       <c r="J185" s="2"/>
-      <c r="K185" s="4"/>
+      <c r="K185" s="2" t="s">
+        <v>457</v>
+      </c>
     </row>
     <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
@@ -14139,7 +14145,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="201" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
         <v>137</v>
       </c>
@@ -14164,7 +14170,7 @@
       </c>
       <c r="K201" s="4"/>
     </row>
-    <row r="202" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
         <v>137</v>
       </c>
@@ -14187,7 +14193,7 @@
       <c r="J202" s="2"/>
       <c r="K202" s="4"/>
     </row>
-    <row r="203" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
         <v>137</v>
       </c>
@@ -14212,7 +14218,7 @@
       <c r="J203" s="2"/>
       <c r="K203" s="4"/>
     </row>
-    <row r="204" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
         <v>137</v>
       </c>
@@ -14239,7 +14245,7 @@
       <c r="J204" s="2"/>
       <c r="K204" s="4"/>
     </row>
-    <row r="205" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>137</v>
       </c>
@@ -14266,7 +14272,7 @@
       <c r="J205" s="2"/>
       <c r="K205" s="4"/>
     </row>
-    <row r="206" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
         <v>137</v>
       </c>
@@ -14295,7 +14301,7 @@
       </c>
       <c r="K206" s="4"/>
     </row>
-    <row r="207" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
         <v>137</v>
       </c>
@@ -14322,7 +14328,7 @@
       <c r="J207" s="2"/>
       <c r="K207" s="4"/>
     </row>
-    <row r="208" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
         <v>137</v>
       </c>
@@ -14349,7 +14355,7 @@
       <c r="J208" s="2"/>
       <c r="K208" s="4"/>
     </row>
-    <row r="209" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
         <v>137</v>
       </c>
@@ -14376,7 +14382,7 @@
       <c r="J209" s="2"/>
       <c r="K209" s="4"/>
     </row>
-    <row r="210" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>137</v>
       </c>

</xml_diff>